<commit_message>
Refactor threshold value in linesensor.h and adjust buzzer timings in main.cpp
</commit_message>
<xml_diff>
--- a/Assessment 2 v1/Results Waypoint 2.xlsx
+++ b/Assessment 2 v1/Results Waypoint 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/kk19332_bristol_ac_uk/Documents/Documents/Eng Des/Year 5/Robotics-Systems-A2/Assessment 2 v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_15B070DFB61526E87D0EFF6311960E32AC82380C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9130C3F1-3F56-438D-B2C3-33523ED3BA7A}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_15B070DFB61526E87D0EFF6311960E32AC82380C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95D0D2C3-D6B3-4A3F-837F-531547437671}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7560" yWindow="1149" windowWidth="19286" windowHeight="12025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Waypoints" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A1:AR11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -587,6 +587,21 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
     <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="AQ1:AR1"/>
     <mergeCell ref="AE1:AF1"/>
@@ -594,21 +609,6 @@
     <mergeCell ref="AI1:AJ1"/>
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished first new wavelength
</commit_message>
<xml_diff>
--- a/Assessment 2 v1/Results Waypoint 2.xlsx
+++ b/Assessment 2 v1/Results Waypoint 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/kk19332_bristol_ac_uk/Documents/Documents/Eng Des/Year 5/Robotics-Systems-A2/Assessment 2 v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="11_15B070DFB61526E87D0EFF6311960E32AC82380C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E06AFF48-7A24-464B-92F6-E5EE4D56E778}"/>
+  <xr:revisionPtr revIDLastSave="300" documentId="11_15B070DFB61526E87D0EFF6311960E32AC82380C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{553BA6BD-B82B-4916-9B27-1501BC63183C}"/>
   <bookViews>
     <workbookView xWindow="3154" yWindow="986" windowWidth="19286" windowHeight="12025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="83">
   <si>
     <t>Square Wave Speed x</t>
   </si>
@@ -153,6 +153,135 @@
   </si>
   <si>
     <t>Square Wave Speed 3 A0.1 W0.4</t>
+  </si>
+  <si>
+    <t>0.23,-0.11</t>
+  </si>
+  <si>
+    <t>0.18,0.09</t>
+  </si>
+  <si>
+    <t>0.20,-0.14</t>
+  </si>
+  <si>
+    <t>0.36,0.02</t>
+  </si>
+  <si>
+    <t>0.37,-0.02</t>
+  </si>
+  <si>
+    <t>0.41,0.14</t>
+  </si>
+  <si>
+    <t>0.39,0.13</t>
+  </si>
+  <si>
+    <t>0.40,0.14</t>
+  </si>
+  <si>
+    <t>0.36,-0.03</t>
+  </si>
+  <si>
+    <t>0.38,0.13</t>
+  </si>
+  <si>
+    <t>0.44,0.10</t>
+  </si>
+  <si>
+    <t>0.16,0.02</t>
+  </si>
+  <si>
+    <t>0.21,0.06</t>
+  </si>
+  <si>
+    <t>0.21,-0.02</t>
+  </si>
+  <si>
+    <t>0.43,0.12</t>
+  </si>
+  <si>
+    <t>0.43,0.11</t>
+  </si>
+  <si>
+    <t>0.40,0.13</t>
+  </si>
+  <si>
+    <t>Square Wave Speed 1 A0.1 W0.2</t>
+  </si>
+  <si>
+    <t>0.11,0.04</t>
+  </si>
+  <si>
+    <t>0.10,-0.06</t>
+  </si>
+  <si>
+    <t>0.23,-0.02</t>
+  </si>
+  <si>
+    <t>0.19,0.07</t>
+  </si>
+  <si>
+    <t>0.29,0.04</t>
+  </si>
+  <si>
+    <t>0.28,0.04</t>
+  </si>
+  <si>
+    <t>0.32,-0.03</t>
+  </si>
+  <si>
+    <t>0.19,0.06</t>
+  </si>
+  <si>
+    <t>0.29,0.03</t>
+  </si>
+  <si>
+    <t>0.11,-0.06</t>
+  </si>
+  <si>
+    <t>0.20,0.07</t>
+  </si>
+  <si>
+    <t>0.22,-0.02</t>
+  </si>
+  <si>
+    <t>0.16,0.03</t>
+  </si>
+  <si>
+    <t>0.22,-0.10</t>
+  </si>
+  <si>
+    <t>0.28,0.03</t>
+  </si>
+  <si>
+    <t>0.11,0.05</t>
+  </si>
+  <si>
+    <t>0.31,-0.02</t>
+  </si>
+  <si>
+    <t>0.32,-0.02</t>
+  </si>
+  <si>
+    <t>0.31,-0.03</t>
+  </si>
+  <si>
+    <t>0.23,-0.03</t>
+  </si>
+  <si>
+    <t>0.31,-0.04</t>
+  </si>
+  <si>
+    <t>0.11,-0.05</t>
+  </si>
+  <si>
+    <t>0.32,-0.01</t>
+  </si>
+  <si>
+    <t>0.30,-0.14</t>
+  </si>
+  <si>
+    <t>0.38,0.01</t>
   </si>
 </sst>
 </file>
@@ -207,13 +336,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,10 +647,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:BD32"/>
+  <dimension ref="A1:DC32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="BD2" sqref="BD2:BD16"/>
+    <sheetView tabSelected="1" topLeftCell="CC1" zoomScale="61" workbookViewId="0">
+      <selection activeCell="DC17" sqref="DC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -534,7 +662,7 @@
     <col min="29" max="45" width="13.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:107" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -543,36 +671,39 @@
         <v>10</v>
       </c>
       <c r="D1" s="1"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
       <c r="AC1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
       <c r="BD1" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="CE1" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:107" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>9.4E-2</v>
       </c>
@@ -735,8 +866,158 @@
       <c r="BD2" t="s">
         <v>33</v>
       </c>
+      <c r="BE2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>41</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>59</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>73</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>73</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>73</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>59</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:107" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>0.105</v>
       </c>
@@ -899,8 +1180,158 @@
       <c r="BD3" t="s">
         <v>32</v>
       </c>
+      <c r="BE3" t="s">
+        <v>37</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>32</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>11</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>37</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>32</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>32</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>32</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>32</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>13</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>32</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>37</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>51</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>37</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>53</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>32</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>32</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>37</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>11</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>53</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>38</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>67</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CJ3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CL3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CO3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CP3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CQ3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CU3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CV3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CW3" t="s">
+        <v>67</v>
+      </c>
+      <c r="CX3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CY3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CZ3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DA3" t="s">
+        <v>38</v>
+      </c>
+      <c r="DB3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DC3" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:107" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>0.13699999999999998</v>
       </c>
@@ -1063,8 +1494,158 @@
       <c r="BD4" t="s">
         <v>5</v>
       </c>
+      <c r="BE4" t="s">
+        <v>40</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>23</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>23</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>5</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>29</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>8</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>5</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>8</v>
+      </c>
+      <c r="BO4" t="s">
+        <v>5</v>
+      </c>
+      <c r="BP4" t="s">
+        <v>5</v>
+      </c>
+      <c r="BQ4" t="s">
+        <v>5</v>
+      </c>
+      <c r="BR4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BS4" t="s">
+        <v>5</v>
+      </c>
+      <c r="BT4" t="s">
+        <v>48</v>
+      </c>
+      <c r="BU4" t="s">
+        <v>37</v>
+      </c>
+      <c r="BV4" t="s">
+        <v>40</v>
+      </c>
+      <c r="BW4" t="s">
+        <v>11</v>
+      </c>
+      <c r="BX4" t="s">
+        <v>54</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>5</v>
+      </c>
+      <c r="BZ4" t="s">
+        <v>5</v>
+      </c>
+      <c r="CA4" t="s">
+        <v>8</v>
+      </c>
+      <c r="CB4" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>48</v>
+      </c>
+      <c r="CE4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CF4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CG4" t="s">
+        <v>60</v>
+      </c>
+      <c r="CH4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CI4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CJ4" t="s">
+        <v>71</v>
+      </c>
+      <c r="CK4" t="s">
+        <v>5</v>
+      </c>
+      <c r="CL4" t="s">
+        <v>5</v>
+      </c>
+      <c r="CM4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CN4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CO4" t="s">
+        <v>5</v>
+      </c>
+      <c r="CP4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CQ4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CR4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CS4" t="s">
+        <v>71</v>
+      </c>
+      <c r="CT4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CU4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CV4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CW4" t="s">
+        <v>5</v>
+      </c>
+      <c r="CX4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CY4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CZ4" t="s">
+        <v>38</v>
+      </c>
+      <c r="DA4" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB4" t="s">
+        <v>38</v>
+      </c>
+      <c r="DC4" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:107" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>0.18</v>
       </c>
@@ -1227,8 +1808,158 @@
       <c r="BD5" t="s">
         <v>7</v>
       </c>
+      <c r="BE5" t="s">
+        <v>29</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>23</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>43</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>8</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>46</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>28</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>47</v>
+      </c>
+      <c r="BO5" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP5" t="s">
+        <v>23</v>
+      </c>
+      <c r="BQ5" t="s">
+        <v>23</v>
+      </c>
+      <c r="BR5" t="s">
+        <v>12</v>
+      </c>
+      <c r="BS5" t="s">
+        <v>29</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>49</v>
+      </c>
+      <c r="BU5" t="s">
+        <v>40</v>
+      </c>
+      <c r="BV5" t="s">
+        <v>29</v>
+      </c>
+      <c r="BW5" t="s">
+        <v>28</v>
+      </c>
+      <c r="BX5" t="s">
+        <v>49</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ5" t="s">
+        <v>23</v>
+      </c>
+      <c r="CA5" t="s">
+        <v>56</v>
+      </c>
+      <c r="CB5" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC5" t="s">
+        <v>50</v>
+      </c>
+      <c r="CE5" t="s">
+        <v>60</v>
+      </c>
+      <c r="CF5" t="s">
+        <v>60</v>
+      </c>
+      <c r="CG5" t="s">
+        <v>65</v>
+      </c>
+      <c r="CH5" t="s">
+        <v>60</v>
+      </c>
+      <c r="CI5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CJ5" t="s">
+        <v>60</v>
+      </c>
+      <c r="CK5" t="s">
+        <v>38</v>
+      </c>
+      <c r="CL5" t="s">
+        <v>37</v>
+      </c>
+      <c r="CM5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CN5" t="s">
+        <v>60</v>
+      </c>
+      <c r="CO5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CP5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CQ5" t="s">
+        <v>60</v>
+      </c>
+      <c r="CR5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CS5" t="s">
+        <v>22</v>
+      </c>
+      <c r="CT5" t="s">
+        <v>60</v>
+      </c>
+      <c r="CU5" t="s">
+        <v>60</v>
+      </c>
+      <c r="CV5" t="s">
+        <v>60</v>
+      </c>
+      <c r="CW5" t="s">
+        <v>38</v>
+      </c>
+      <c r="CX5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CY5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CZ5" t="s">
+        <v>60</v>
+      </c>
+      <c r="DA5" t="s">
+        <v>65</v>
+      </c>
+      <c r="DB5" t="s">
+        <v>22</v>
+      </c>
+      <c r="DC5" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:107" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>0.21299999999999999</v>
       </c>
@@ -1391,8 +2122,158 @@
       <c r="BD6" t="s">
         <v>9</v>
       </c>
+      <c r="BE6" t="s">
+        <v>8</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>8</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BQ6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT6" t="s">
+        <v>50</v>
+      </c>
+      <c r="BU6" t="s">
+        <v>8</v>
+      </c>
+      <c r="BV6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ6" t="s">
+        <v>55</v>
+      </c>
+      <c r="CA6" t="s">
+        <v>9</v>
+      </c>
+      <c r="CB6" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC6" t="s">
+        <v>46</v>
+      </c>
+      <c r="CE6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CF6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CG6" t="s">
+        <v>66</v>
+      </c>
+      <c r="CH6" t="s">
+        <v>68</v>
+      </c>
+      <c r="CI6" t="s">
+        <v>70</v>
+      </c>
+      <c r="CJ6" t="s">
+        <v>65</v>
+      </c>
+      <c r="CK6" t="s">
+        <v>69</v>
+      </c>
+      <c r="CL6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CM6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CN6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CO6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CP6" t="s">
+        <v>51</v>
+      </c>
+      <c r="CQ6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CR6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CS6" t="s">
+        <v>65</v>
+      </c>
+      <c r="CT6" t="s">
+        <v>68</v>
+      </c>
+      <c r="CU6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CV6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CW6" t="s">
+        <v>69</v>
+      </c>
+      <c r="CX6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CY6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CZ6" t="s">
+        <v>65</v>
+      </c>
+      <c r="DA6" t="s">
+        <v>78</v>
+      </c>
+      <c r="DB6" t="s">
+        <v>61</v>
+      </c>
+      <c r="DC6" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:107" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>0.22399999999999998</v>
       </c>
@@ -1555,8 +2436,158 @@
       <c r="BD7" t="s">
         <v>9</v>
       </c>
+      <c r="BE7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>45</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BQ7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU7" t="s">
+        <v>47</v>
+      </c>
+      <c r="BV7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ7" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA7" t="s">
+        <v>9</v>
+      </c>
+      <c r="CB7" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC7" t="s">
+        <v>9</v>
+      </c>
+      <c r="CE7" t="s">
+        <v>62</v>
+      </c>
+      <c r="CF7" t="s">
+        <v>63</v>
+      </c>
+      <c r="CG7" t="s">
+        <v>44</v>
+      </c>
+      <c r="CH7" t="s">
+        <v>66</v>
+      </c>
+      <c r="CI7" t="s">
+        <v>61</v>
+      </c>
+      <c r="CJ7" t="s">
+        <v>72</v>
+      </c>
+      <c r="CK7" t="s">
+        <v>61</v>
+      </c>
+      <c r="CL7" t="s">
+        <v>74</v>
+      </c>
+      <c r="CM7" t="s">
+        <v>62</v>
+      </c>
+      <c r="CN7" t="s">
+        <v>62</v>
+      </c>
+      <c r="CO7" t="s">
+        <v>62</v>
+      </c>
+      <c r="CP7" t="s">
+        <v>68</v>
+      </c>
+      <c r="CQ7" t="s">
+        <v>64</v>
+      </c>
+      <c r="CR7" t="s">
+        <v>62</v>
+      </c>
+      <c r="CS7" t="s">
+        <v>76</v>
+      </c>
+      <c r="CT7" t="s">
+        <v>76</v>
+      </c>
+      <c r="CU7" t="s">
+        <v>62</v>
+      </c>
+      <c r="CV7" t="s">
+        <v>76</v>
+      </c>
+      <c r="CW7" t="s">
+        <v>61</v>
+      </c>
+      <c r="CX7" t="s">
+        <v>63</v>
+      </c>
+      <c r="CY7" t="s">
+        <v>76</v>
+      </c>
+      <c r="CZ7" t="s">
+        <v>66</v>
+      </c>
+      <c r="DA7" t="s">
+        <v>44</v>
+      </c>
+      <c r="DB7" t="s">
+        <v>62</v>
+      </c>
+      <c r="DC7" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:107" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>0.26700000000000002</v>
       </c>
@@ -1719,8 +2750,158 @@
       <c r="BD8" t="s">
         <v>9</v>
       </c>
+      <c r="BE8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BQ8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ8" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA8" t="s">
+        <v>9</v>
+      </c>
+      <c r="CB8" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC8" t="s">
+        <v>9</v>
+      </c>
+      <c r="CE8" t="s">
+        <v>29</v>
+      </c>
+      <c r="CF8" t="s">
+        <v>64</v>
+      </c>
+      <c r="CG8" t="s">
+        <v>9</v>
+      </c>
+      <c r="CH8" t="s">
+        <v>64</v>
+      </c>
+      <c r="CI8" t="s">
+        <v>7</v>
+      </c>
+      <c r="CJ8" t="s">
+        <v>64</v>
+      </c>
+      <c r="CK8" t="s">
+        <v>7</v>
+      </c>
+      <c r="CL8" t="s">
+        <v>28</v>
+      </c>
+      <c r="CM8" t="s">
+        <v>64</v>
+      </c>
+      <c r="CN8" t="s">
+        <v>75</v>
+      </c>
+      <c r="CO8" t="s">
+        <v>75</v>
+      </c>
+      <c r="CP8" t="s">
+        <v>64</v>
+      </c>
+      <c r="CQ8" t="s">
+        <v>29</v>
+      </c>
+      <c r="CR8" t="s">
+        <v>75</v>
+      </c>
+      <c r="CS8" t="s">
+        <v>9</v>
+      </c>
+      <c r="CT8" t="s">
+        <v>9</v>
+      </c>
+      <c r="CU8" t="s">
+        <v>64</v>
+      </c>
+      <c r="CV8" t="s">
+        <v>9</v>
+      </c>
+      <c r="CW8" t="s">
+        <v>75</v>
+      </c>
+      <c r="CX8" t="s">
+        <v>75</v>
+      </c>
+      <c r="CY8" t="s">
+        <v>29</v>
+      </c>
+      <c r="CZ8" t="s">
+        <v>64</v>
+      </c>
+      <c r="DA8" t="s">
+        <v>9</v>
+      </c>
+      <c r="DB8" t="s">
+        <v>76</v>
+      </c>
+      <c r="DC8" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:107" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>0.29899999999999999</v>
       </c>
@@ -1883,8 +3064,158 @@
       <c r="BD9" t="s">
         <v>9</v>
       </c>
+      <c r="BE9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BQ9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CB9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CE9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CF9" t="s">
+        <v>29</v>
+      </c>
+      <c r="CG9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CH9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CI9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CJ9" t="s">
+        <v>44</v>
+      </c>
+      <c r="CK9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CL9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CM9" t="s">
+        <v>29</v>
+      </c>
+      <c r="CN9" t="s">
+        <v>29</v>
+      </c>
+      <c r="CO9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CP9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CQ9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CR9" t="s">
+        <v>29</v>
+      </c>
+      <c r="CS9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CT9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CU9" t="s">
+        <v>29</v>
+      </c>
+      <c r="CV9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CW9" t="s">
+        <v>7</v>
+      </c>
+      <c r="CX9" t="s">
+        <v>29</v>
+      </c>
+      <c r="CY9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CZ9" t="s">
+        <v>29</v>
+      </c>
+      <c r="DA9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DB9" t="s">
+        <v>29</v>
+      </c>
+      <c r="DC9" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:107" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>0.33200000000000002</v>
       </c>
@@ -2047,8 +3378,158 @@
       <c r="BD10" t="s">
         <v>9</v>
       </c>
+      <c r="BE10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BQ10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CB10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CE10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CF10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CG10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CH10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CI10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CJ10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CK10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CL10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CM10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CN10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CO10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CP10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CQ10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CR10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CS10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CT10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CU10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CV10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CW10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CX10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CY10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CZ10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DA10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DB10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DC10" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:107" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>0.35399999999999998</v>
       </c>
@@ -2211,8 +3692,158 @@
       <c r="BD11" t="s">
         <v>9</v>
       </c>
+      <c r="BE11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BQ11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY11" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CB11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CE11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CF11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CG11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CH11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CI11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CJ11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CK11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CL11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CM11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CN11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CO11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CP11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CQ11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CR11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CS11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CT11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CU11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CV11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CW11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CX11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CY11" t="s">
+        <v>9</v>
+      </c>
+      <c r="CZ11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DA11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DB11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DC11" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:107" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
         <v>9</v>
       </c>
@@ -2369,8 +4000,158 @@
       <c r="BD12" t="s">
         <v>9</v>
       </c>
+      <c r="BE12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BQ12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY12" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CB12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CE12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CF12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CG12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CH12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CI12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CJ12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CK12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CL12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CM12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CN12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CO12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CP12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CQ12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CR12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CS12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CT12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CU12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CV12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CW12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CX12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CY12" t="s">
+        <v>9</v>
+      </c>
+      <c r="CZ12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DA12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DB12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DC12" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:107" x14ac:dyDescent="0.4">
       <c r="C13" t="s">
         <v>9</v>
       </c>
@@ -2527,8 +4308,158 @@
       <c r="BD13" t="s">
         <v>9</v>
       </c>
+      <c r="BE13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BQ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CB13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CE13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CF13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CG13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CH13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CI13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CJ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CK13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CL13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CM13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CN13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CO13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CP13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CQ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CR13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CS13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CT13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CU13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CV13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CW13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CX13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CY13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CZ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DA13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DB13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DC13" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:107" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
         <v>9</v>
       </c>
@@ -2685,8 +4616,158 @@
       <c r="BD14" t="s">
         <v>9</v>
       </c>
+      <c r="BE14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BQ14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CB14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CE14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CF14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CG14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CH14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CI14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CJ14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CK14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CL14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CM14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CN14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CO14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CP14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CQ14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CR14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CS14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CT14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CU14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CV14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CW14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CX14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CY14" t="s">
+        <v>9</v>
+      </c>
+      <c r="CZ14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DA14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DB14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DC14" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:107" x14ac:dyDescent="0.4">
       <c r="C15" t="s">
         <v>9</v>
       </c>
@@ -2843,8 +4924,158 @@
       <c r="BD15" t="s">
         <v>9</v>
       </c>
+      <c r="BE15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BQ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CB15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CE15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CF15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CG15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CH15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CI15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CJ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CK15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CL15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CM15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CN15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CO15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CP15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CQ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CR15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CS15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CT15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CU15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CV15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CW15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CX15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CY15" t="s">
+        <v>9</v>
+      </c>
+      <c r="CZ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DA15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DB15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DC15" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:107" x14ac:dyDescent="0.4">
       <c r="C16" t="s">
         <v>9</v>
       </c>
@@ -3001,8 +5232,158 @@
       <c r="BD16" t="s">
         <v>9</v>
       </c>
+      <c r="BE16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BQ16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CB16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CE16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CF16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CG16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CH16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CI16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CJ16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CK16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CL16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CM16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CN16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CO16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CP16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CQ16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CR16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CS16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CT16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CU16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CV16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CW16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CX16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CY16" t="s">
+        <v>9</v>
+      </c>
+      <c r="CZ16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DA16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DB16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DC16" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="17" spans="2:54" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:107" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -3159,56 +5540,209 @@
       <c r="BB17">
         <v>15257</v>
       </c>
+      <c r="BD17">
+        <v>11110</v>
+      </c>
+      <c r="BE17">
+        <v>12103</v>
+      </c>
+      <c r="BF17">
+        <v>12612</v>
+      </c>
+      <c r="BG17">
+        <v>12594</v>
+      </c>
+      <c r="BH17">
+        <v>14063</v>
+      </c>
+      <c r="BI17">
+        <v>14880</v>
+      </c>
+      <c r="BJ17">
+        <v>13968</v>
+      </c>
+      <c r="BK17">
+        <v>14504</v>
+      </c>
+      <c r="BL17">
+        <v>11481</v>
+      </c>
+      <c r="BM17">
+        <v>11547</v>
+      </c>
+      <c r="BN17">
+        <v>11042</v>
+      </c>
+      <c r="BO17">
+        <v>11209</v>
+      </c>
+      <c r="BP17">
+        <v>11240</v>
+      </c>
+      <c r="BQ17">
+        <v>12475</v>
+      </c>
+      <c r="BR17">
+        <v>11762</v>
+      </c>
+      <c r="BS17">
+        <v>11604</v>
+      </c>
+      <c r="BT17">
+        <v>11679</v>
+      </c>
+      <c r="BU17">
+        <v>12481</v>
+      </c>
+      <c r="BV17">
+        <v>11728</v>
+      </c>
+      <c r="BW17">
+        <v>11085</v>
+      </c>
+      <c r="BX17">
+        <v>11155</v>
+      </c>
+      <c r="BY17">
+        <v>11168</v>
+      </c>
+      <c r="BZ17">
+        <v>11894</v>
+      </c>
+      <c r="CA17">
+        <v>11242</v>
+      </c>
+      <c r="CB17">
+        <v>10897</v>
+      </c>
+      <c r="CC17">
+        <v>11094</v>
+      </c>
+      <c r="CE17">
+        <v>37842</v>
+      </c>
+      <c r="CF17">
+        <v>38296</v>
+      </c>
+      <c r="CG17">
+        <v>37144</v>
+      </c>
+      <c r="CH17">
+        <v>39723</v>
+      </c>
+      <c r="CI17">
+        <v>35253</v>
+      </c>
+      <c r="CJ17">
+        <v>41887</v>
+      </c>
+      <c r="CK17">
+        <v>37159</v>
+      </c>
+      <c r="CL17">
+        <v>37910</v>
+      </c>
+      <c r="CM17">
+        <v>35372</v>
+      </c>
+      <c r="CN17">
+        <v>37053</v>
+      </c>
+      <c r="CO17">
+        <v>38631</v>
+      </c>
+      <c r="CP17">
+        <v>37080</v>
+      </c>
+      <c r="CQ17">
+        <v>38630</v>
+      </c>
+      <c r="CR17">
+        <v>38646</v>
+      </c>
+      <c r="CS17">
+        <v>38879</v>
+      </c>
+      <c r="CT17">
+        <v>37867</v>
+      </c>
+      <c r="CU17">
+        <v>37371</v>
+      </c>
+      <c r="CV17">
+        <v>37963</v>
+      </c>
+      <c r="CW17">
+        <v>41129</v>
+      </c>
+      <c r="CX17">
+        <v>39086</v>
+      </c>
+      <c r="CY17">
+        <v>36877</v>
+      </c>
+      <c r="CZ17">
+        <v>35280</v>
+      </c>
+      <c r="DA17">
+        <v>35595</v>
+      </c>
+      <c r="DB17">
+        <v>37827</v>
+      </c>
+      <c r="DC17">
+        <v>37036</v>
+      </c>
     </row>
-    <row r="22" spans="2:54" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:107" x14ac:dyDescent="0.4">
       <c r="C22" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="2:54" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:107" x14ac:dyDescent="0.4">
       <c r="C23" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:54" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:107" x14ac:dyDescent="0.4">
       <c r="C24" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:54" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:107" x14ac:dyDescent="0.4">
       <c r="C25" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:54" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:107" x14ac:dyDescent="0.4">
       <c r="C26" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:54" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:107" x14ac:dyDescent="0.4">
       <c r="C27" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:54" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:107" x14ac:dyDescent="0.4">
       <c r="C28" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:54" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:107" x14ac:dyDescent="0.4">
       <c r="C29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="32" spans="2:54" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:107" x14ac:dyDescent="0.4">
       <c r="C32" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Completed initial runs on square wave
</commit_message>
<xml_diff>
--- a/Assessment 2 v1/Results Waypoint 2.xlsx
+++ b/Assessment 2 v1/Results Waypoint 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/kk19332_bristol_ac_uk/Documents/Documents/Eng Des/Year 5/Robotics-Systems-A2/Assessment 2 v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="300" documentId="11_15B070DFB61526E87D0EFF6311960E32AC82380C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{553BA6BD-B82B-4916-9B27-1501BC63183C}"/>
+  <xr:revisionPtr revIDLastSave="410" documentId="11_15B070DFB61526E87D0EFF6311960E32AC82380C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C924A3F-6783-44B7-AE2B-99CD76966BBA}"/>
   <bookViews>
-    <workbookView xWindow="3154" yWindow="986" windowWidth="19286" windowHeight="12025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3497" yWindow="1329" windowWidth="19286" windowHeight="12025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Waypoints" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2297" uniqueCount="114">
   <si>
     <t>Square Wave Speed x</t>
   </si>
@@ -282,6 +282,99 @@
   </si>
   <si>
     <t>0.38,0.01</t>
+  </si>
+  <si>
+    <t>Square Wave Speed 2 A0.1 W0.2</t>
+  </si>
+  <si>
+    <t>0.12,0.04</t>
+  </si>
+  <si>
+    <t>0.09,-0.06</t>
+  </si>
+  <si>
+    <t>0.30,-0.04</t>
+  </si>
+  <si>
+    <t>0.18,0.06</t>
+  </si>
+  <si>
+    <t>0.27,0.04</t>
+  </si>
+  <si>
+    <t>0.22,-0.11</t>
+  </si>
+  <si>
+    <t>0.10,-0.05</t>
+  </si>
+  <si>
+    <t>0.36,-0.02</t>
+  </si>
+  <si>
+    <t>0.19,0.08</t>
+  </si>
+  <si>
+    <t>0.27,0.05</t>
+  </si>
+  <si>
+    <t>0.31,-0.14</t>
+  </si>
+  <si>
+    <t>0.18,0.08</t>
+  </si>
+  <si>
+    <t>0.28,0.06</t>
+  </si>
+  <si>
+    <t>0.31,-0.01</t>
+  </si>
+  <si>
+    <t>0.29,-0.13</t>
+  </si>
+  <si>
+    <t>0.34,-0.14</t>
+  </si>
+  <si>
+    <t>0.30,-0.03</t>
+  </si>
+  <si>
+    <t>0.13,0.03</t>
+  </si>
+  <si>
+    <t>Square Wave Speed 3 A0.1 W0.2</t>
+  </si>
+  <si>
+    <t>0.21,-0.10</t>
+  </si>
+  <si>
+    <t>0.30,-0.02</t>
+  </si>
+  <si>
+    <t>0.27,0.03</t>
+  </si>
+  <si>
+    <t>0.10,0.04</t>
+  </si>
+  <si>
+    <t>0.44,0.09</t>
+  </si>
+  <si>
+    <t>0.44,0.13</t>
+  </si>
+  <si>
+    <t>0.45,0.11</t>
+  </si>
+  <si>
+    <t>0.22,-0.03</t>
+  </si>
+  <si>
+    <t>0.10,-0.07</t>
+  </si>
+  <si>
+    <t>0.20,0.06</t>
+  </si>
+  <si>
+    <t>0.37,-0.03</t>
   </si>
 </sst>
 </file>
@@ -647,10 +740,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:DC32"/>
+  <dimension ref="A1:FC32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CC1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="DC17" sqref="DC17"/>
+    <sheetView tabSelected="1" topLeftCell="EA1" zoomScale="62" workbookViewId="0">
+      <selection activeCell="EK7" sqref="EK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -662,7 +755,7 @@
     <col min="29" max="45" width="13.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:107" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:159" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -702,8 +795,14 @@
       <c r="CE1" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="DE1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="EE1" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="2" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:159" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>9.4E-2</v>
       </c>
@@ -1016,8 +1115,158 @@
       <c r="DC2" t="s">
         <v>73</v>
       </c>
+      <c r="DE2" t="s">
+        <v>84</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>73</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>73</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>59</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>84</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>58</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>73</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>73</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>73</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>73</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>73</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>73</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>73</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>58</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>106</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>73</v>
+      </c>
+      <c r="ET2" t="s">
+        <v>73</v>
+      </c>
+      <c r="EU2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EV2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EX2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EY2" t="s">
+        <v>58</v>
+      </c>
+      <c r="EZ2" t="s">
+        <v>73</v>
+      </c>
+      <c r="FA2" t="s">
+        <v>58</v>
+      </c>
+      <c r="FB2" t="s">
+        <v>58</v>
+      </c>
+      <c r="FC2" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="3" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:159" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>0.105</v>
       </c>
@@ -1330,8 +1579,158 @@
       <c r="DC3" t="s">
         <v>79</v>
       </c>
+      <c r="DE3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DF3" t="s">
+        <v>85</v>
+      </c>
+      <c r="DG3" t="s">
+        <v>85</v>
+      </c>
+      <c r="DH3" t="s">
+        <v>67</v>
+      </c>
+      <c r="DI3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DJ3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DK3" t="s">
+        <v>71</v>
+      </c>
+      <c r="DL3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DM3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DN3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DO3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DP3" t="s">
+        <v>85</v>
+      </c>
+      <c r="DQ3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DR3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DS3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DT3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DU3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DV3" t="s">
+        <v>90</v>
+      </c>
+      <c r="DW3" t="s">
+        <v>59</v>
+      </c>
+      <c r="DX3" t="s">
+        <v>90</v>
+      </c>
+      <c r="DY3" t="s">
+        <v>90</v>
+      </c>
+      <c r="DZ3" t="s">
+        <v>59</v>
+      </c>
+      <c r="EA3" t="s">
+        <v>101</v>
+      </c>
+      <c r="EB3" t="s">
+        <v>85</v>
+      </c>
+      <c r="EC3" t="s">
+        <v>85</v>
+      </c>
+      <c r="EE3" t="s">
+        <v>85</v>
+      </c>
+      <c r="EF3" t="s">
+        <v>59</v>
+      </c>
+      <c r="EG3" t="s">
+        <v>85</v>
+      </c>
+      <c r="EH3" t="s">
+        <v>101</v>
+      </c>
+      <c r="EI3" t="s">
+        <v>31</v>
+      </c>
+      <c r="EJ3" t="s">
+        <v>59</v>
+      </c>
+      <c r="EK3" t="s">
+        <v>59</v>
+      </c>
+      <c r="EL3" t="s">
+        <v>59</v>
+      </c>
+      <c r="EM3" t="s">
+        <v>101</v>
+      </c>
+      <c r="EN3" t="s">
+        <v>71</v>
+      </c>
+      <c r="EO3" t="s">
+        <v>59</v>
+      </c>
+      <c r="EP3" t="s">
+        <v>59</v>
+      </c>
+      <c r="EQ3" t="s">
+        <v>71</v>
+      </c>
+      <c r="ER3" t="s">
+        <v>85</v>
+      </c>
+      <c r="ES3" t="s">
+        <v>59</v>
+      </c>
+      <c r="ET3" t="s">
+        <v>59</v>
+      </c>
+      <c r="EU3" t="s">
+        <v>59</v>
+      </c>
+      <c r="EV3" t="s">
+        <v>59</v>
+      </c>
+      <c r="EW3" t="s">
+        <v>85</v>
+      </c>
+      <c r="EX3" t="s">
+        <v>59</v>
+      </c>
+      <c r="EY3" t="s">
+        <v>59</v>
+      </c>
+      <c r="EZ3" t="s">
+        <v>90</v>
+      </c>
+      <c r="FA3" t="s">
+        <v>111</v>
+      </c>
+      <c r="FB3" t="s">
+        <v>85</v>
+      </c>
+      <c r="FC3" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="4" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:159" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>0.13699999999999998</v>
       </c>
@@ -1644,8 +2043,158 @@
       <c r="DC4" t="s">
         <v>5</v>
       </c>
+      <c r="DE4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DF4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DG4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DH4" t="s">
+        <v>5</v>
+      </c>
+      <c r="DI4" t="s">
+        <v>5</v>
+      </c>
+      <c r="DJ4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DK4" t="s">
+        <v>69</v>
+      </c>
+      <c r="DL4" t="s">
+        <v>38</v>
+      </c>
+      <c r="DM4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DN4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DO4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DP4" t="s">
+        <v>89</v>
+      </c>
+      <c r="DQ4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DR4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DS4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DT4" t="s">
+        <v>89</v>
+      </c>
+      <c r="DU4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DV4" t="s">
+        <v>31</v>
+      </c>
+      <c r="DW4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DX4" t="s">
+        <v>5</v>
+      </c>
+      <c r="DY4" t="s">
+        <v>5</v>
+      </c>
+      <c r="DZ4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EA4" t="s">
+        <v>85</v>
+      </c>
+      <c r="EB4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EC4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EE4" t="s">
+        <v>103</v>
+      </c>
+      <c r="EF4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EG4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EH4" t="s">
+        <v>85</v>
+      </c>
+      <c r="EI4" t="s">
+        <v>3</v>
+      </c>
+      <c r="EJ4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EK4" t="s">
+        <v>31</v>
+      </c>
+      <c r="EL4" t="s">
+        <v>38</v>
+      </c>
+      <c r="EM4" t="s">
+        <v>85</v>
+      </c>
+      <c r="EN4" t="s">
+        <v>61</v>
+      </c>
+      <c r="EO4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EP4" t="s">
+        <v>38</v>
+      </c>
+      <c r="EQ4" t="s">
+        <v>61</v>
+      </c>
+      <c r="ER4" t="s">
+        <v>71</v>
+      </c>
+      <c r="ES4" t="s">
+        <v>31</v>
+      </c>
+      <c r="ET4" t="s">
+        <v>31</v>
+      </c>
+      <c r="EU4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EV4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EW4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EX4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EY4" t="s">
+        <v>5</v>
+      </c>
+      <c r="EZ4" t="s">
+        <v>5</v>
+      </c>
+      <c r="FA4" t="s">
+        <v>89</v>
+      </c>
+      <c r="FB4" t="s">
+        <v>71</v>
+      </c>
+      <c r="FC4" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="5" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:159" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>0.18</v>
       </c>
@@ -1958,8 +2507,158 @@
       <c r="DC5" t="s">
         <v>22</v>
       </c>
+      <c r="DE5" t="s">
+        <v>69</v>
+      </c>
+      <c r="DF5" t="s">
+        <v>53</v>
+      </c>
+      <c r="DG5" t="s">
+        <v>69</v>
+      </c>
+      <c r="DH5" t="s">
+        <v>61</v>
+      </c>
+      <c r="DI5" t="s">
+        <v>61</v>
+      </c>
+      <c r="DJ5" t="s">
+        <v>61</v>
+      </c>
+      <c r="DK5" t="s">
+        <v>61</v>
+      </c>
+      <c r="DL5" t="s">
+        <v>65</v>
+      </c>
+      <c r="DM5" t="s">
+        <v>53</v>
+      </c>
+      <c r="DN5" t="s">
+        <v>37</v>
+      </c>
+      <c r="DO5" t="s">
+        <v>65</v>
+      </c>
+      <c r="DP5" t="s">
+        <v>53</v>
+      </c>
+      <c r="DQ5" t="s">
+        <v>37</v>
+      </c>
+      <c r="DR5" t="s">
+        <v>32</v>
+      </c>
+      <c r="DS5" t="s">
+        <v>61</v>
+      </c>
+      <c r="DT5" t="s">
+        <v>53</v>
+      </c>
+      <c r="DU5" t="s">
+        <v>65</v>
+      </c>
+      <c r="DV5" t="s">
+        <v>61</v>
+      </c>
+      <c r="DW5" t="s">
+        <v>53</v>
+      </c>
+      <c r="DX5" t="s">
+        <v>92</v>
+      </c>
+      <c r="DY5" t="s">
+        <v>37</v>
+      </c>
+      <c r="DZ5" t="s">
+        <v>3</v>
+      </c>
+      <c r="EA5" t="s">
+        <v>71</v>
+      </c>
+      <c r="EB5" t="s">
+        <v>32</v>
+      </c>
+      <c r="EC5" t="s">
+        <v>32</v>
+      </c>
+      <c r="EE5" t="s">
+        <v>53</v>
+      </c>
+      <c r="EF5" t="s">
+        <v>3</v>
+      </c>
+      <c r="EG5" t="s">
+        <v>87</v>
+      </c>
+      <c r="EH5" t="s">
+        <v>71</v>
+      </c>
+      <c r="EI5" t="s">
+        <v>93</v>
+      </c>
+      <c r="EJ5" t="s">
+        <v>87</v>
+      </c>
+      <c r="EK5" t="s">
+        <v>93</v>
+      </c>
+      <c r="EL5" t="s">
+        <v>61</v>
+      </c>
+      <c r="EM5" t="s">
+        <v>71</v>
+      </c>
+      <c r="EN5" t="s">
+        <v>76</v>
+      </c>
+      <c r="EO5" t="s">
+        <v>32</v>
+      </c>
+      <c r="EP5" t="s">
+        <v>61</v>
+      </c>
+      <c r="EQ5" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER5" t="s">
+        <v>53</v>
+      </c>
+      <c r="ES5" t="s">
+        <v>61</v>
+      </c>
+      <c r="ET5" t="s">
+        <v>37</v>
+      </c>
+      <c r="EU5" t="s">
+        <v>65</v>
+      </c>
+      <c r="EV5" t="s">
+        <v>61</v>
+      </c>
+      <c r="EW5" t="s">
+        <v>65</v>
+      </c>
+      <c r="EX5" t="s">
+        <v>110</v>
+      </c>
+      <c r="EY5" t="s">
+        <v>38</v>
+      </c>
+      <c r="EZ5" t="s">
+        <v>61</v>
+      </c>
+      <c r="FA5" t="s">
+        <v>112</v>
+      </c>
+      <c r="FB5" t="s">
+        <v>65</v>
+      </c>
+      <c r="FC5" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="6" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:159" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>0.21299999999999999</v>
       </c>
@@ -2272,8 +2971,158 @@
       <c r="DC6" t="s">
         <v>61</v>
       </c>
+      <c r="DE6" t="s">
+        <v>65</v>
+      </c>
+      <c r="DF6" t="s">
+        <v>65</v>
+      </c>
+      <c r="DG6" t="s">
+        <v>87</v>
+      </c>
+      <c r="DH6" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI6" t="s">
+        <v>74</v>
+      </c>
+      <c r="DJ6" t="s">
+        <v>29</v>
+      </c>
+      <c r="DK6" t="s">
+        <v>76</v>
+      </c>
+      <c r="DL6" t="s">
+        <v>76</v>
+      </c>
+      <c r="DM6" t="s">
+        <v>65</v>
+      </c>
+      <c r="DN6" t="s">
+        <v>61</v>
+      </c>
+      <c r="DO6" t="s">
+        <v>76</v>
+      </c>
+      <c r="DP6" t="s">
+        <v>65</v>
+      </c>
+      <c r="DQ6" t="s">
+        <v>61</v>
+      </c>
+      <c r="DR6" t="s">
+        <v>61</v>
+      </c>
+      <c r="DS6" t="s">
+        <v>29</v>
+      </c>
+      <c r="DT6" t="s">
+        <v>65</v>
+      </c>
+      <c r="DU6" t="s">
+        <v>76</v>
+      </c>
+      <c r="DV6" t="s">
+        <v>74</v>
+      </c>
+      <c r="DW6" t="s">
+        <v>65</v>
+      </c>
+      <c r="DX6" t="s">
+        <v>93</v>
+      </c>
+      <c r="DY6" t="s">
+        <v>95</v>
+      </c>
+      <c r="DZ6" t="s">
+        <v>93</v>
+      </c>
+      <c r="EA6" t="s">
+        <v>69</v>
+      </c>
+      <c r="EB6" t="s">
+        <v>93</v>
+      </c>
+      <c r="EC6" t="s">
+        <v>61</v>
+      </c>
+      <c r="EE6" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF6" t="s">
+        <v>104</v>
+      </c>
+      <c r="EG6" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH6" t="s">
+        <v>65</v>
+      </c>
+      <c r="EI6" t="s">
+        <v>74</v>
+      </c>
+      <c r="EJ6" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK6" t="s">
+        <v>74</v>
+      </c>
+      <c r="EL6" t="s">
+        <v>74</v>
+      </c>
+      <c r="EM6" t="s">
+        <v>53</v>
+      </c>
+      <c r="EN6" t="s">
+        <v>44</v>
+      </c>
+      <c r="EO6" t="s">
+        <v>65</v>
+      </c>
+      <c r="EP6" t="s">
+        <v>76</v>
+      </c>
+      <c r="EQ6" t="s">
+        <v>74</v>
+      </c>
+      <c r="ER6" t="s">
+        <v>61</v>
+      </c>
+      <c r="ES6" t="s">
+        <v>62</v>
+      </c>
+      <c r="ET6" t="s">
+        <v>61</v>
+      </c>
+      <c r="EU6" t="s">
+        <v>88</v>
+      </c>
+      <c r="EV6" t="s">
+        <v>76</v>
+      </c>
+      <c r="EW6" t="s">
+        <v>76</v>
+      </c>
+      <c r="EX6" t="s">
+        <v>61</v>
+      </c>
+      <c r="EY6" t="s">
+        <v>61</v>
+      </c>
+      <c r="EZ6" t="s">
+        <v>62</v>
+      </c>
+      <c r="FA6" t="s">
+        <v>78</v>
+      </c>
+      <c r="FB6" t="s">
+        <v>78</v>
+      </c>
+      <c r="FC6" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="7" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:159" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>0.22399999999999998</v>
       </c>
@@ -2586,8 +3435,158 @@
       <c r="DC7" t="s">
         <v>80</v>
       </c>
+      <c r="DE7" t="s">
+        <v>76</v>
+      </c>
+      <c r="DF7" t="s">
+        <v>86</v>
+      </c>
+      <c r="DG7" t="s">
+        <v>72</v>
+      </c>
+      <c r="DH7" t="s">
+        <v>74</v>
+      </c>
+      <c r="DI7" t="s">
+        <v>28</v>
+      </c>
+      <c r="DJ7" t="s">
+        <v>9</v>
+      </c>
+      <c r="DK7" t="s">
+        <v>29</v>
+      </c>
+      <c r="DL7" t="s">
+        <v>23</v>
+      </c>
+      <c r="DM7" t="s">
+        <v>29</v>
+      </c>
+      <c r="DN7" t="s">
+        <v>76</v>
+      </c>
+      <c r="DO7" t="s">
+        <v>29</v>
+      </c>
+      <c r="DP7" t="s">
+        <v>78</v>
+      </c>
+      <c r="DQ7" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR7" t="s">
+        <v>7</v>
+      </c>
+      <c r="DS7" t="s">
+        <v>9</v>
+      </c>
+      <c r="DT7" t="s">
+        <v>44</v>
+      </c>
+      <c r="DU7" t="s">
+        <v>29</v>
+      </c>
+      <c r="DV7" t="s">
+        <v>7</v>
+      </c>
+      <c r="DW7" t="s">
+        <v>72</v>
+      </c>
+      <c r="DX7" t="s">
+        <v>74</v>
+      </c>
+      <c r="DY7" t="s">
+        <v>96</v>
+      </c>
+      <c r="DZ7" t="s">
+        <v>100</v>
+      </c>
+      <c r="EA7" t="s">
+        <v>87</v>
+      </c>
+      <c r="EB7" t="s">
+        <v>74</v>
+      </c>
+      <c r="EC7" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE7" t="s">
+        <v>100</v>
+      </c>
+      <c r="EF7" t="s">
+        <v>54</v>
+      </c>
+      <c r="EG7" t="s">
+        <v>100</v>
+      </c>
+      <c r="EH7" t="s">
+        <v>105</v>
+      </c>
+      <c r="EI7" t="s">
+        <v>28</v>
+      </c>
+      <c r="EJ7" t="s">
+        <v>100</v>
+      </c>
+      <c r="EK7" t="s">
+        <v>28</v>
+      </c>
+      <c r="EL7" t="s">
+        <v>7</v>
+      </c>
+      <c r="EM7" t="s">
+        <v>61</v>
+      </c>
+      <c r="EN7" t="s">
+        <v>9</v>
+      </c>
+      <c r="EO7" t="s">
+        <v>76</v>
+      </c>
+      <c r="EP7" t="s">
+        <v>44</v>
+      </c>
+      <c r="EQ7" t="s">
+        <v>7</v>
+      </c>
+      <c r="ER7" t="s">
+        <v>88</v>
+      </c>
+      <c r="ES7" t="s">
+        <v>75</v>
+      </c>
+      <c r="ET7" t="s">
+        <v>75</v>
+      </c>
+      <c r="EU7" t="s">
+        <v>76</v>
+      </c>
+      <c r="EV7" t="s">
+        <v>29</v>
+      </c>
+      <c r="EW7" t="s">
+        <v>29</v>
+      </c>
+      <c r="EX7" t="s">
+        <v>76</v>
+      </c>
+      <c r="EY7" t="s">
+        <v>7</v>
+      </c>
+      <c r="EZ7" t="s">
+        <v>75</v>
+      </c>
+      <c r="FA7" t="s">
+        <v>113</v>
+      </c>
+      <c r="FB7" t="s">
+        <v>44</v>
+      </c>
+      <c r="FC7" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="8" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:159" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>0.26700000000000002</v>
       </c>
@@ -2900,8 +3899,158 @@
       <c r="DC8" t="s">
         <v>81</v>
       </c>
+      <c r="DE8" t="s">
+        <v>29</v>
+      </c>
+      <c r="DF8" t="s">
+        <v>29</v>
+      </c>
+      <c r="DG8" t="s">
+        <v>44</v>
+      </c>
+      <c r="DH8" t="s">
+        <v>7</v>
+      </c>
+      <c r="DI8" t="s">
+        <v>9</v>
+      </c>
+      <c r="DJ8" t="s">
+        <v>9</v>
+      </c>
+      <c r="DK8" t="s">
+        <v>9</v>
+      </c>
+      <c r="DL8" t="s">
+        <v>9</v>
+      </c>
+      <c r="DM8" t="s">
+        <v>9</v>
+      </c>
+      <c r="DN8" t="s">
+        <v>29</v>
+      </c>
+      <c r="DO8" t="s">
+        <v>9</v>
+      </c>
+      <c r="DP8" t="s">
+        <v>44</v>
+      </c>
+      <c r="DQ8" t="s">
+        <v>74</v>
+      </c>
+      <c r="DR8" t="s">
+        <v>9</v>
+      </c>
+      <c r="DS8" t="s">
+        <v>9</v>
+      </c>
+      <c r="DT8" t="s">
+        <v>8</v>
+      </c>
+      <c r="DU8" t="s">
+        <v>9</v>
+      </c>
+      <c r="DV8" t="s">
+        <v>9</v>
+      </c>
+      <c r="DW8" t="s">
+        <v>64</v>
+      </c>
+      <c r="DX8" t="s">
+        <v>94</v>
+      </c>
+      <c r="DY8" t="s">
+        <v>97</v>
+      </c>
+      <c r="DZ8" t="s">
+        <v>15</v>
+      </c>
+      <c r="EA8" t="s">
+        <v>88</v>
+      </c>
+      <c r="EB8" t="s">
+        <v>15</v>
+      </c>
+      <c r="EC8" t="s">
+        <v>100</v>
+      </c>
+      <c r="EE8" t="s">
+        <v>55</v>
+      </c>
+      <c r="EF8" t="s">
+        <v>9</v>
+      </c>
+      <c r="EG8" t="s">
+        <v>23</v>
+      </c>
+      <c r="EH8" t="s">
+        <v>91</v>
+      </c>
+      <c r="EI8" t="s">
+        <v>9</v>
+      </c>
+      <c r="EJ8" t="s">
+        <v>29</v>
+      </c>
+      <c r="EK8" t="s">
+        <v>9</v>
+      </c>
+      <c r="EL8" t="s">
+        <v>9</v>
+      </c>
+      <c r="EM8" t="s">
+        <v>72</v>
+      </c>
+      <c r="EN8" t="s">
+        <v>9</v>
+      </c>
+      <c r="EO8" t="s">
+        <v>29</v>
+      </c>
+      <c r="EP8" t="s">
+        <v>9</v>
+      </c>
+      <c r="EQ8" t="s">
+        <v>9</v>
+      </c>
+      <c r="ER8" t="s">
+        <v>76</v>
+      </c>
+      <c r="ES8" t="s">
+        <v>7</v>
+      </c>
+      <c r="ET8" t="s">
+        <v>28</v>
+      </c>
+      <c r="EU8" t="s">
+        <v>29</v>
+      </c>
+      <c r="EV8" t="s">
+        <v>9</v>
+      </c>
+      <c r="EW8" t="s">
+        <v>9</v>
+      </c>
+      <c r="EX8" t="s">
+        <v>44</v>
+      </c>
+      <c r="EY8" t="s">
+        <v>9</v>
+      </c>
+      <c r="EZ8" t="s">
+        <v>9</v>
+      </c>
+      <c r="FA8" t="s">
+        <v>46</v>
+      </c>
+      <c r="FB8" t="s">
+        <v>9</v>
+      </c>
+      <c r="FC8" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="9" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:159" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>0.29899999999999999</v>
       </c>
@@ -3214,8 +4363,158 @@
       <c r="DC9" t="s">
         <v>82</v>
       </c>
+      <c r="DE9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DF9" t="s">
+        <v>8</v>
+      </c>
+      <c r="DG9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DH9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DI9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DJ9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DK9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DL9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DM9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DN9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DO9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DP9" t="s">
+        <v>50</v>
+      </c>
+      <c r="DQ9" t="s">
+        <v>29</v>
+      </c>
+      <c r="DR9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DS9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DT9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DU9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DV9" t="s">
+        <v>9</v>
+      </c>
+      <c r="DW9" t="s">
+        <v>91</v>
+      </c>
+      <c r="DX9" t="s">
+        <v>27</v>
+      </c>
+      <c r="DY9" t="s">
+        <v>98</v>
+      </c>
+      <c r="DZ9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EA9" t="s">
+        <v>100</v>
+      </c>
+      <c r="EB9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EC9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EE9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EF9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EG9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EH9" t="s">
+        <v>47</v>
+      </c>
+      <c r="EI9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EJ9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EK9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EL9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EM9" t="s">
+        <v>23</v>
+      </c>
+      <c r="EN9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EO9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EP9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EQ9" t="s">
+        <v>9</v>
+      </c>
+      <c r="ER9" t="s">
+        <v>29</v>
+      </c>
+      <c r="ES9" t="s">
+        <v>9</v>
+      </c>
+      <c r="ET9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EU9" t="s">
+        <v>107</v>
+      </c>
+      <c r="EV9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EW9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EX9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EY9" t="s">
+        <v>9</v>
+      </c>
+      <c r="EZ9" t="s">
+        <v>9</v>
+      </c>
+      <c r="FA9" t="s">
+        <v>9</v>
+      </c>
+      <c r="FB9" t="s">
+        <v>9</v>
+      </c>
+      <c r="FC9" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="10" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:159" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>0.33200000000000002</v>
       </c>
@@ -3528,8 +4827,158 @@
       <c r="DC10" t="s">
         <v>9</v>
       </c>
+      <c r="DE10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DF10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DG10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DH10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DI10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DJ10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DK10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DL10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DM10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DN10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DO10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DP10" t="s">
+        <v>45</v>
+      </c>
+      <c r="DQ10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DR10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DS10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DT10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DU10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DV10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DW10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DX10" t="s">
+        <v>9</v>
+      </c>
+      <c r="DY10" t="s">
+        <v>99</v>
+      </c>
+      <c r="DZ10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EA10" t="s">
+        <v>55</v>
+      </c>
+      <c r="EB10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EC10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EE10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EF10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EG10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EH10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EI10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EJ10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EK10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EL10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EM10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EN10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EO10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EP10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EQ10" t="s">
+        <v>9</v>
+      </c>
+      <c r="ER10" t="s">
+        <v>9</v>
+      </c>
+      <c r="ES10" t="s">
+        <v>9</v>
+      </c>
+      <c r="ET10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EU10" t="s">
+        <v>45</v>
+      </c>
+      <c r="EV10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EW10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EX10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EY10" t="s">
+        <v>9</v>
+      </c>
+      <c r="EZ10" t="s">
+        <v>9</v>
+      </c>
+      <c r="FA10" t="s">
+        <v>9</v>
+      </c>
+      <c r="FB10" t="s">
+        <v>9</v>
+      </c>
+      <c r="FC10" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="11" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:159" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>0.35399999999999998</v>
       </c>
@@ -3842,8 +5291,158 @@
       <c r="DC11" t="s">
         <v>9</v>
       </c>
+      <c r="DE11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DF11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DG11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DH11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DI11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DJ11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DK11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DL11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DM11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DN11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DO11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DP11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DQ11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DR11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DS11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DT11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DU11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DV11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DW11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DX11" t="s">
+        <v>9</v>
+      </c>
+      <c r="DY11" t="s">
+        <v>25</v>
+      </c>
+      <c r="DZ11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EA11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EB11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EC11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EE11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EF11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EG11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EH11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EI11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EJ11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EK11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EL11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EM11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EN11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EO11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EP11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EQ11" t="s">
+        <v>9</v>
+      </c>
+      <c r="ER11" t="s">
+        <v>9</v>
+      </c>
+      <c r="ES11" t="s">
+        <v>9</v>
+      </c>
+      <c r="ET11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EU11" t="s">
+        <v>108</v>
+      </c>
+      <c r="EV11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EW11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EX11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EY11" t="s">
+        <v>9</v>
+      </c>
+      <c r="EZ11" t="s">
+        <v>9</v>
+      </c>
+      <c r="FA11" t="s">
+        <v>9</v>
+      </c>
+      <c r="FB11" t="s">
+        <v>9</v>
+      </c>
+      <c r="FC11" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:159" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
         <v>9</v>
       </c>
@@ -4150,8 +5749,158 @@
       <c r="DC12" t="s">
         <v>9</v>
       </c>
+      <c r="DE12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DF12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DG12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DH12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DI12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DJ12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DK12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DL12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DM12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DN12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DO12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DP12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DQ12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DR12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DS12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DT12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DU12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DV12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DW12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DX12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DY12" t="s">
+        <v>9</v>
+      </c>
+      <c r="DZ12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EA12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EB12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EC12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EE12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EF12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EG12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EH12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EI12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EJ12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EK12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EL12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EM12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EN12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EO12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EP12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EQ12" t="s">
+        <v>9</v>
+      </c>
+      <c r="ER12" t="s">
+        <v>9</v>
+      </c>
+      <c r="ES12" t="s">
+        <v>9</v>
+      </c>
+      <c r="ET12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EU12" t="s">
+        <v>109</v>
+      </c>
+      <c r="EV12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EW12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EX12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EY12" t="s">
+        <v>9</v>
+      </c>
+      <c r="EZ12" t="s">
+        <v>9</v>
+      </c>
+      <c r="FA12" t="s">
+        <v>9</v>
+      </c>
+      <c r="FB12" t="s">
+        <v>9</v>
+      </c>
+      <c r="FC12" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="13" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:159" x14ac:dyDescent="0.4">
       <c r="C13" t="s">
         <v>9</v>
       </c>
@@ -4458,8 +6207,158 @@
       <c r="DC13" t="s">
         <v>9</v>
       </c>
+      <c r="DE13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DF13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DG13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DH13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DI13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DJ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DK13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DL13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DM13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DN13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DO13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DP13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DQ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DR13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DS13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DT13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DU13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DV13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DW13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DX13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DY13" t="s">
+        <v>9</v>
+      </c>
+      <c r="DZ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EA13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EB13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EC13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EE13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EF13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EG13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EH13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EI13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EJ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EK13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EL13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EM13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EN13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EO13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EP13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EQ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="ER13" t="s">
+        <v>9</v>
+      </c>
+      <c r="ES13" t="s">
+        <v>9</v>
+      </c>
+      <c r="ET13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EU13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EV13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EW13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EX13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EY13" t="s">
+        <v>9</v>
+      </c>
+      <c r="EZ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="FA13" t="s">
+        <v>9</v>
+      </c>
+      <c r="FB13" t="s">
+        <v>9</v>
+      </c>
+      <c r="FC13" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="14" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:159" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
         <v>9</v>
       </c>
@@ -4766,8 +6665,158 @@
       <c r="DC14" t="s">
         <v>9</v>
       </c>
+      <c r="DE14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DF14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DG14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DH14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DI14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DJ14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DK14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DL14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DM14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DN14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DO14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DP14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DQ14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DR14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DS14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DT14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DU14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DV14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DW14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DX14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DY14" t="s">
+        <v>9</v>
+      </c>
+      <c r="DZ14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EA14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EB14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EC14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EE14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EF14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EG14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EH14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EI14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EJ14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EK14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EL14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EM14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EN14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EO14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EP14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EQ14" t="s">
+        <v>9</v>
+      </c>
+      <c r="ER14" t="s">
+        <v>9</v>
+      </c>
+      <c r="ES14" t="s">
+        <v>9</v>
+      </c>
+      <c r="ET14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EU14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EV14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EW14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EX14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EY14" t="s">
+        <v>9</v>
+      </c>
+      <c r="EZ14" t="s">
+        <v>9</v>
+      </c>
+      <c r="FA14" t="s">
+        <v>9</v>
+      </c>
+      <c r="FB14" t="s">
+        <v>9</v>
+      </c>
+      <c r="FC14" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="15" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:159" x14ac:dyDescent="0.4">
       <c r="C15" t="s">
         <v>9</v>
       </c>
@@ -5074,8 +7123,158 @@
       <c r="DC15" t="s">
         <v>9</v>
       </c>
+      <c r="DE15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DF15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DG15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DH15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DI15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DJ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DK15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DL15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DM15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DN15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DO15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DP15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DQ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DR15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DS15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DT15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DU15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DV15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DW15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DX15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DY15" t="s">
+        <v>9</v>
+      </c>
+      <c r="DZ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EA15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EB15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EC15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EE15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EF15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EG15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EH15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EI15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EJ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EK15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EL15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EM15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EN15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EO15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EP15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EQ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="ER15" t="s">
+        <v>9</v>
+      </c>
+      <c r="ES15" t="s">
+        <v>9</v>
+      </c>
+      <c r="ET15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EU15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EV15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EW15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EX15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EY15" t="s">
+        <v>9</v>
+      </c>
+      <c r="EZ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="FA15" t="s">
+        <v>9</v>
+      </c>
+      <c r="FB15" t="s">
+        <v>9</v>
+      </c>
+      <c r="FC15" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="16" spans="1:107" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:159" x14ac:dyDescent="0.4">
       <c r="C16" t="s">
         <v>9</v>
       </c>
@@ -5382,8 +7581,158 @@
       <c r="DC16" t="s">
         <v>9</v>
       </c>
+      <c r="DE16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DF16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DG16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DH16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DI16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DJ16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DK16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DL16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DM16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DN16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DO16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DP16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DQ16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DR16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DS16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DT16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DU16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DV16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DW16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DX16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DY16" t="s">
+        <v>9</v>
+      </c>
+      <c r="DZ16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EA16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EB16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EC16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EE16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EF16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EG16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EH16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EI16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EJ16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EK16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EL16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EM16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EN16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EO16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EP16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EQ16" t="s">
+        <v>9</v>
+      </c>
+      <c r="ER16" t="s">
+        <v>9</v>
+      </c>
+      <c r="ES16" t="s">
+        <v>9</v>
+      </c>
+      <c r="ET16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EU16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EV16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EW16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EX16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EY16" t="s">
+        <v>9</v>
+      </c>
+      <c r="EZ16" t="s">
+        <v>9</v>
+      </c>
+      <c r="FA16" t="s">
+        <v>9</v>
+      </c>
+      <c r="FB16" t="s">
+        <v>9</v>
+      </c>
+      <c r="FC16" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="17" spans="2:107" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:159" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -5693,56 +8042,206 @@
       <c r="DC17">
         <v>37036</v>
       </c>
+      <c r="DE17">
+        <v>25131</v>
+      </c>
+      <c r="DF17">
+        <v>24023</v>
+      </c>
+      <c r="DG17">
+        <v>27256</v>
+      </c>
+      <c r="DH17">
+        <v>24242</v>
+      </c>
+      <c r="DI17">
+        <v>23506</v>
+      </c>
+      <c r="DJ17">
+        <v>23777</v>
+      </c>
+      <c r="DK17">
+        <v>23557</v>
+      </c>
+      <c r="DL17">
+        <v>22794</v>
+      </c>
+      <c r="DM17">
+        <v>23413</v>
+      </c>
+      <c r="DN17">
+        <v>23262</v>
+      </c>
+      <c r="DO17">
+        <v>23365</v>
+      </c>
+      <c r="DP17">
+        <v>22598</v>
+      </c>
+      <c r="DQ17">
+        <v>24670</v>
+      </c>
+      <c r="DR17">
+        <v>23249</v>
+      </c>
+      <c r="DS17">
+        <v>22882</v>
+      </c>
+      <c r="DT17">
+        <v>24091</v>
+      </c>
+      <c r="DU17">
+        <v>24346</v>
+      </c>
+      <c r="DV17">
+        <v>26399</v>
+      </c>
+      <c r="DW17">
+        <v>24067</v>
+      </c>
+      <c r="DX17">
+        <v>23604</v>
+      </c>
+      <c r="DY17">
+        <v>24176</v>
+      </c>
+      <c r="DZ17">
+        <v>24736</v>
+      </c>
+      <c r="EA17">
+        <v>23467</v>
+      </c>
+      <c r="EB17">
+        <v>24387</v>
+      </c>
+      <c r="EC17">
+        <v>23287</v>
+      </c>
+      <c r="EE17">
+        <v>17183</v>
+      </c>
+      <c r="EF17">
+        <v>18199</v>
+      </c>
+      <c r="EG17">
+        <v>17266</v>
+      </c>
+      <c r="EH17">
+        <v>20750</v>
+      </c>
+      <c r="EI17">
+        <v>17041</v>
+      </c>
+      <c r="EJ17">
+        <v>19638</v>
+      </c>
+      <c r="EK17">
+        <v>17157</v>
+      </c>
+      <c r="EL17">
+        <v>17250</v>
+      </c>
+      <c r="EM17">
+        <v>18847</v>
+      </c>
+      <c r="EN17">
+        <v>17732</v>
+      </c>
+      <c r="EO17">
+        <v>17206</v>
+      </c>
+      <c r="EP17">
+        <v>18066</v>
+      </c>
+      <c r="EQ17">
+        <v>18953</v>
+      </c>
+      <c r="ER17">
+        <v>18632</v>
+      </c>
+      <c r="ES17">
+        <v>18816</v>
+      </c>
+      <c r="ET17">
+        <v>20457</v>
+      </c>
+      <c r="EU17">
+        <v>18640</v>
+      </c>
+      <c r="EV17">
+        <v>18683</v>
+      </c>
+      <c r="EW17">
+        <v>19109</v>
+      </c>
+      <c r="EX17">
+        <v>20605</v>
+      </c>
+      <c r="EY17">
+        <v>19598</v>
+      </c>
+      <c r="EZ17">
+        <v>23191</v>
+      </c>
+      <c r="FA17">
+        <v>19450</v>
+      </c>
+      <c r="FB17">
+        <v>19844</v>
+      </c>
+      <c r="FC17">
+        <v>20646</v>
+      </c>
     </row>
-    <row r="22" spans="2:107" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:159" x14ac:dyDescent="0.4">
       <c r="C22" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="2:107" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:159" x14ac:dyDescent="0.4">
       <c r="C23" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:107" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:159" x14ac:dyDescent="0.4">
       <c r="C24" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:107" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:159" x14ac:dyDescent="0.4">
       <c r="C25" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:107" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:159" x14ac:dyDescent="0.4">
       <c r="C26" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:107" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:159" x14ac:dyDescent="0.4">
       <c r="C27" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:107" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:159" x14ac:dyDescent="0.4">
       <c r="C28" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:107" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:159" x14ac:dyDescent="0.4">
       <c r="C29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="32" spans="2:107" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:159" x14ac:dyDescent="0.4">
       <c r="C32" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>